<commit_message>
Modified the Document Action_Plans_for_learning.xlsx
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\2_GIT_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EDCB9E-67ED-487D-BA2F-DCE9BF52E9EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F111DDB4-3202-4298-9ECD-6DAE00852AA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="0" windowWidth="19650" windowHeight="7875" tabRatio="554" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="554" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_Career PATH" sheetId="36" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="262">
   <si>
     <t>SR#</t>
   </si>
@@ -2611,6 +2611,41 @@
       </rPr>
       <t xml:space="preserve"> Story Board, Task Board, Burndown Charts &amp; Member Dashboard
 (9.22 mins)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>V1 Free Trial Link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.collab.net/products/versionone-editions</t>
     </r>
   </si>
 </sst>
@@ -2875,7 +2910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3083,12 +3118,90 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3104,83 +3217,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3743,10 +3781,10 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,31 +3792,31 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="42.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="61" customWidth="1"/>
-    <col min="4" max="4" width="67.140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.140625" style="79" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="23" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -3802,32 +3840,32 @@
       <c r="A4" s="63">
         <v>1</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="83" t="s">
         <v>233</v>
       </c>
       <c r="C4" s="61" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="74" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
-      <c r="B5" s="91"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="74" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
+    <row r="6" spans="1:6" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -3836,139 +3874,139 @@
       <c r="B7" s="63" t="s">
         <v>225</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="73" t="s">
         <v>226</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="74" t="s">
         <v>221</v>
       </c>
       <c r="E7" s="72"/>
-      <c r="F7" s="83"/>
+      <c r="F7" s="75"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="73" t="s">
         <v>227</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="74" t="s">
         <v>222</v>
       </c>
       <c r="E8" s="69"/>
-      <c r="F8" s="83"/>
+      <c r="F8" s="75"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="74" t="s">
         <v>223</v>
       </c>
       <c r="E9" s="69"/>
-      <c r="F9" s="83"/>
+      <c r="F9" s="75"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="73" t="s">
         <v>229</v>
       </c>
-      <c r="D10" s="82" t="s">
+      <c r="D10" s="74" t="s">
         <v>224</v>
       </c>
       <c r="E10" s="69"/>
-      <c r="F10" s="83"/>
-    </row>
-    <row r="11" spans="1:6" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="96"/>
-      <c r="B11" s="96"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="100"/>
+      <c r="F10" s="75"/>
+    </row>
+    <row r="11" spans="1:6" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="92"/>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>3</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="80" t="s">
         <v>231</v>
       </c>
-      <c r="D12" s="82" t="s">
+      <c r="D12" s="74" t="s">
         <v>230</v>
       </c>
       <c r="E12" s="69"/>
-      <c r="F12" s="83"/>
-    </row>
-    <row r="13" spans="1:6" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="100"/>
+      <c r="F12" s="75"/>
+    </row>
+    <row r="13" spans="1:6" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="88"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>4</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="74" t="s">
         <v>230</v>
       </c>
       <c r="E14" s="69"/>
-      <c r="F14" s="83"/>
+      <c r="F14" s="75"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="89"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="67" t="s">
         <v>239</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="74" t="s">
         <v>234</v>
       </c>
       <c r="E15" s="69"/>
-      <c r="F15" s="83"/>
+      <c r="F15" s="75"/>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="84" t="s">
+      <c r="B16" s="81"/>
+      <c r="C16" s="76" t="s">
         <v>236</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="D16" s="74" t="s">
         <v>237</v>
       </c>
       <c r="E16" s="69"/>
-      <c r="F16" s="83"/>
+      <c r="F16" s="75"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="85"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="69"/>
-      <c r="F17" s="83"/>
+      <c r="F17" s="75"/>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="96" t="s">
         <v>240</v>
       </c>
-      <c r="C18" s="105" t="s">
+      <c r="C18" s="97" t="s">
         <v>252</v>
       </c>
-      <c r="D18" s="82" t="s">
+      <c r="D18" s="74" t="s">
         <v>241</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -3976,98 +4014,101 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="103" t="s">
+      <c r="B19" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="C19" s="105" t="s">
+      <c r="C19" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="D19" s="82" t="s">
+      <c r="D19" s="74" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="95" t="s">
         <v>245</v>
       </c>
-      <c r="C20" s="105" t="s">
+      <c r="C20" s="97" t="s">
         <v>254</v>
       </c>
-      <c r="D20" s="82" t="s">
+      <c r="D20" s="74" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C21" s="105" t="s">
+      <c r="B21" s="106" t="s">
+        <v>261</v>
+      </c>
+      <c r="C21" s="97" t="s">
         <v>255</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="D21" s="74" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="C22" s="105" t="s">
+      <c r="C22" s="97" t="s">
         <v>256</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D22" s="74" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="90"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="105" t="s">
+      <c r="A23" s="82"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="97" t="s">
         <v>260</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="D23" s="74" t="s">
         <v>248</v>
       </c>
       <c r="E23" s="69"/>
-      <c r="F23" s="83"/>
+      <c r="F23" s="75"/>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="90"/>
-      <c r="C24" s="105" t="s">
+      <c r="A24" s="82"/>
+      <c r="C24" s="97" t="s">
         <v>257</v>
       </c>
-      <c r="D24" s="82" t="s">
+      <c r="D24" s="74" t="s">
         <v>249</v>
       </c>
       <c r="E24" s="69"/>
-      <c r="F24" s="83"/>
+      <c r="F24" s="75"/>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="90"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="105" t="s">
+      <c r="A25" s="82"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="97" t="s">
         <v>258</v>
       </c>
-      <c r="D25" s="82" t="s">
+      <c r="D25" s="74" t="s">
         <v>250</v>
       </c>
       <c r="E25" s="69"/>
-      <c r="F25" s="83"/>
+      <c r="F25" s="75"/>
     </row>
     <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="C26" s="105" t="s">
+      <c r="C26" s="97" t="s">
         <v>259</v>
       </c>
-      <c r="D26" s="82" t="s">
+      <c r="D26" s="74" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="84"/>
+      <c r="C27" s="76"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
@@ -4076,7 +4117,7 @@
       <c r="B29" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="86" t="s">
+      <c r="C29" s="78" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="14" t="s">
@@ -4093,7 +4134,7 @@
       <c r="B30" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="87"/>
+      <c r="C30" s="79"/>
       <c r="D30" s="1" t="s">
         <v>29</v>
       </c>
@@ -4106,7 +4147,7 @@
       <c r="B31" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="87"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="1" t="s">
         <v>30</v>
       </c>
@@ -4119,7 +4160,7 @@
       <c r="B32" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="87"/>
+      <c r="C32" s="79"/>
       <c r="D32" s="1" t="s">
         <v>30</v>
       </c>
@@ -4182,14 +4223,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4252,14 +4293,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4322,14 +4363,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4392,14 +4433,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4462,14 +4503,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4532,14 +4573,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4602,14 +4643,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4673,12 +4714,12 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
     </row>
@@ -4705,11 +4746,11 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="103" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
       <c r="E3" s="39" t="s">
         <v>149</v>
       </c>
@@ -5005,12 +5046,12 @@
       <c r="A1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
       <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5036,11 +5077,11 @@
       <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="104" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
       <c r="E3" s="48" t="s">
         <v>150</v>
       </c>
@@ -5117,11 +5158,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="104" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="48" t="s">
         <v>150</v>
       </c>
@@ -5272,7 +5313,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5285,22 +5326,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -5621,13 +5662,13 @@
       <c r="E26" s="71"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
@@ -5786,28 +5827,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -6132,16 +6173,16 @@
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="99"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
@@ -6273,14 +6314,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6340,14 +6381,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6412,14 +6453,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6482,13 +6523,13 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -6631,14 +6672,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6701,14 +6742,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6751,6 +6792,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d53f460e102142885dbc8938524af06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" xmlns:ns4="c8965576-7528-46e3-a68d-d4bc5141fdaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51dd3132ab51039a0b8a02bab29c14ac" ns3:_="" ns4:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -6973,22 +7029,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
+    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC42E61D-1BC2-43F5-95E9-ABDA8B3BC8C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7005,29 +7071,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
-    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Scrum Agile Docs
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\2_GIT_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A7BC76-79CE-46DE-AF1A-96581457D78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9711C175-D4F6-4B25-B65C-AA94974552AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="554" activeTab="3" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="554" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_Career PATH" sheetId="36" r:id="rId1"/>
@@ -38,7 +38,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Career PATH'!$A$3:$H$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Primary_Career PATH'!$A$3:$F$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Primary_Career PATH'!$A$3:$F$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Secondary_Career PATH'!$A$3:$E$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="285">
   <si>
     <t>SR#</t>
   </si>
@@ -2694,12 +2694,177 @@
   <si>
     <t>Open</t>
   </si>
+  <si>
+    <t>Coaching</t>
+  </si>
+  <si>
+    <t>Managing</t>
+  </si>
+  <si>
+    <t>Practicing</t>
+  </si>
+  <si>
+    <t>Leading</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Beginner:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Getting Started</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intermediate:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Executing a Team Iteration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intermediate:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Executing a Program Increament</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intermediate:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Running a Large Solution at Scale</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intermediate:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Managing the Delivery Portfolio</t>
+    </r>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/executing-team-iteration</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/managing-delivery-portfolio</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/executing-program-increment</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/running-large-solution-at-scale</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Advanced:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Advanced Topics in Scaling Agile</t>
+    </r>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/scaling-agile-advanced-topics</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2881,8 +3046,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2961,8 +3134,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2985,12 +3164,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3273,12 +3489,63 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3294,37 +3561,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3885,20 +4125,20 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="42.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39" style="61" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="61" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.140625" style="78" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="23" customWidth="1"/>
@@ -3906,30 +4146,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="111"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="52" t="s">
         <v>1</v>
       </c>
@@ -3943,7 +4183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63">
         <v>1</v>
       </c>
@@ -3985,8 +4225,10 @@
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="108" t="s">
+      <c r="B8" s="107" t="s">
+        <v>270</v>
+      </c>
+      <c r="C8" s="100" t="s">
         <v>226</v>
       </c>
       <c r="D8" s="73" t="s">
@@ -3997,13 +4239,13 @@
     <row r="9" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="106" t="s">
-        <v>262</v>
+      <c r="C9" s="122" t="s">
+        <v>274</v>
       </c>
       <c r="D9" s="73" t="s">
         <v>263</v>
       </c>
-      <c r="E9" s="107" t="s">
+      <c r="E9" s="99" t="s">
         <v>267</v>
       </c>
       <c r="F9" s="74"/>
@@ -4011,327 +4253,389 @@
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="87"/>
+      <c r="C10" s="122" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>279</v>
+      </c>
+      <c r="E10" s="123"/>
       <c r="F10" s="74"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="72" t="s">
-        <v>228</v>
+      <c r="C11" s="122" t="s">
+        <v>276</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>223</v>
-      </c>
-      <c r="E11" s="69"/>
+        <v>281</v>
+      </c>
+      <c r="E11" s="123"/>
       <c r="F11" s="74"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="72" t="s">
-        <v>229</v>
+      <c r="C12" s="122" t="s">
+        <v>277</v>
       </c>
       <c r="D12" s="73" t="s">
-        <v>224</v>
-      </c>
-      <c r="E12" s="69"/>
+        <v>282</v>
+      </c>
+      <c r="E12" s="123"/>
       <c r="F12" s="74"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="72" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="73" t="s">
-        <v>222</v>
-      </c>
-      <c r="E13" s="69"/>
+      <c r="C13" s="122" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" s="108" t="s">
+        <v>280</v>
+      </c>
+      <c r="E13" s="81"/>
       <c r="F13" s="74"/>
     </row>
-    <row r="14" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="87"/>
-      <c r="B14" s="87"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="90"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>3</v>
-      </c>
-      <c r="B15" s="80" t="s">
-        <v>232</v>
-      </c>
-      <c r="C15" s="79" t="s">
-        <v>231</v>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="122" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" s="108" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="81"/>
+      <c r="F14" s="74"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="107" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="72" t="s">
+        <v>228</v>
       </c>
       <c r="D15" s="73" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E15" s="69"/>
       <c r="F15" s="74"/>
     </row>
-    <row r="16" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="90"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="107" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>229</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="69"/>
+      <c r="F16" s="74"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>4</v>
-      </c>
-      <c r="B17" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="79" t="s">
-        <v>238</v>
+      <c r="A17" s="11"/>
+      <c r="B17" s="107" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>227</v>
       </c>
       <c r="D17" s="73" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E17" s="69"/>
       <c r="F17" s="74"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="67" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" s="73" t="s">
-        <v>234</v>
-      </c>
-      <c r="E18" s="69"/>
-      <c r="F18" s="74"/>
+    <row r="18" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="87"/>
+      <c r="B18" s="87"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="75" t="s">
-        <v>236</v>
+      <c r="A19" s="11">
+        <v>3</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" s="79" t="s">
+        <v>231</v>
       </c>
       <c r="D19" s="73" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E19" s="69"/>
       <c r="F19" s="74"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="74"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="94" t="s">
+    <row r="20" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="87"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="90"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>4</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="79" t="s">
+        <v>238</v>
+      </c>
+      <c r="D21" s="73" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="69"/>
+      <c r="F21" s="74"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="67" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>234</v>
+      </c>
+      <c r="E22" s="69"/>
+      <c r="F22" s="74"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23" s="73" t="s">
+        <v>237</v>
+      </c>
+      <c r="E23" s="69"/>
+      <c r="F23" s="74"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="74"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="94" t="s">
         <v>240</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C25" s="95" t="s">
         <v>252</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D25" s="73" t="s">
         <v>241</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="93" t="s">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="93" t="s">
         <v>246</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C26" s="95" t="s">
         <v>253</v>
       </c>
-      <c r="D22" s="73" t="s">
+      <c r="D26" s="73" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="93" t="s">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="93" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C27" s="95" t="s">
         <v>254</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="D27" s="73" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="96" t="s">
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C28" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="D24" s="73" t="s">
+      <c r="D28" s="73" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="C25" s="95" t="s">
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="C29" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D25" s="73" t="s">
+      <c r="D29" s="73" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="95" t="s">
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="81"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="95" t="s">
         <v>259</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D30" s="73" t="s">
         <v>248</v>
       </c>
-      <c r="E26" s="69"/>
-      <c r="F26" s="74"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="81"/>
-      <c r="C27" s="95" t="s">
+      <c r="E30" s="69"/>
+      <c r="F30" s="74"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="81"/>
+      <c r="C31" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="D27" s="73" t="s">
+      <c r="D31" s="73" t="s">
         <v>249</v>
       </c>
-      <c r="E27" s="69"/>
-      <c r="F27" s="74"/>
-    </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="95" t="s">
+      <c r="E31" s="69"/>
+      <c r="F31" s="74"/>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="81"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="95" t="s">
         <v>258</v>
       </c>
-      <c r="D28" s="73" t="s">
+      <c r="D32" s="73" t="s">
         <v>250</v>
       </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="74"/>
-    </row>
-    <row r="29" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="C29" s="95" t="s">
+      <c r="E32" s="69"/>
+      <c r="F32" s="74"/>
+    </row>
+    <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="C33" s="95" t="s">
         <v>261</v>
       </c>
-      <c r="D29" s="73" t="s">
+      <c r="D33" s="73" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="75"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="98" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="75"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="B35" s="113"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="113"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
         <v>1</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B36" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C36" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D36" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E36" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>2</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B37" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="78"/>
-      <c r="D33" s="1" t="s">
+      <c r="C37" s="78"/>
+      <c r="D37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="E37" s="23"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>3</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="B38" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="1" t="s">
+      <c r="C38" s="78"/>
+      <c r="D38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="23"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
         <v>4</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B39" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="78"/>
-      <c r="D35" s="1" t="s">
+      <c r="C39" s="78"/>
+      <c r="D39" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E39" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F33" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
+  <autoFilter ref="A3:F37" xr:uid="{D1AE8F92-0427-4F12-8484-D03DDDD5BCBC}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A35:F35"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" xr:uid="{2E23BA7A-5B0B-4DA9-B8B9-53FB09B14F77}"/>
-    <hyperlink ref="D13" r:id="rId2" xr:uid="{E3E6E9E0-714A-4113-84F4-A77A0938F58A}"/>
-    <hyperlink ref="D11" r:id="rId3" xr:uid="{BA2493B0-601A-4F54-9E3A-F5C3A0303CD9}"/>
-    <hyperlink ref="D12" r:id="rId4" xr:uid="{BE536791-6143-4FD8-B898-9135A9957678}"/>
-    <hyperlink ref="D15" r:id="rId5" xr:uid="{B74F90BE-EEF3-4193-A6AB-D1C361C2129C}"/>
-    <hyperlink ref="D17" r:id="rId6" xr:uid="{1E39F6AC-7883-4749-89AA-D035D148D1B4}"/>
-    <hyperlink ref="D18" r:id="rId7" xr:uid="{D8D4679C-3F88-4BD7-9A49-3F9FBFBEFDBC}"/>
+    <hyperlink ref="D17" r:id="rId2" xr:uid="{E3E6E9E0-714A-4113-84F4-A77A0938F58A}"/>
+    <hyperlink ref="D15" r:id="rId3" xr:uid="{BA2493B0-601A-4F54-9E3A-F5C3A0303CD9}"/>
+    <hyperlink ref="D16" r:id="rId4" xr:uid="{BE536791-6143-4FD8-B898-9135A9957678}"/>
+    <hyperlink ref="D19" r:id="rId5" xr:uid="{B74F90BE-EEF3-4193-A6AB-D1C361C2129C}"/>
+    <hyperlink ref="D21" r:id="rId6" xr:uid="{1E39F6AC-7883-4749-89AA-D035D148D1B4}"/>
+    <hyperlink ref="D22" r:id="rId7" xr:uid="{D8D4679C-3F88-4BD7-9A49-3F9FBFBEFDBC}"/>
     <hyperlink ref="D5" r:id="rId8" xr:uid="{DF5DB6BC-C32A-446D-A83F-BBAD2AAAAE42}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{C75CA674-BB0B-4179-9544-633A75106152}"/>
-    <hyperlink ref="D19" r:id="rId10" xr:uid="{DEC581DC-25E8-4D22-85FE-968AA311BC4C}"/>
-    <hyperlink ref="D21" r:id="rId11" xr:uid="{25DFE2B8-7111-42E9-BED2-6FAA0E70689C}"/>
-    <hyperlink ref="D22" r:id="rId12" xr:uid="{2B8A48F5-F547-4C41-BD57-626BC8383E02}"/>
-    <hyperlink ref="D23" r:id="rId13" xr:uid="{7D21E112-C538-4EF1-832F-FADEF8B53DBE}"/>
-    <hyperlink ref="D24" r:id="rId14" xr:uid="{8C7FC700-CCF5-4222-ACD9-9FC734098BD2}"/>
-    <hyperlink ref="B23" r:id="rId15" xr:uid="{48C21483-6CA4-4763-AAB2-890458D45A79}"/>
-    <hyperlink ref="B22" r:id="rId16" xr:uid="{9B31FCF5-B1F7-4954-A0D7-C49F11918E5B}"/>
-    <hyperlink ref="D25" r:id="rId17" xr:uid="{4650665B-2233-495D-9E1E-E2BEBDEA1A78}"/>
-    <hyperlink ref="D26" r:id="rId18" xr:uid="{4D8E8BE5-121B-4C5C-979C-7919982CFF66}"/>
-    <hyperlink ref="D27" r:id="rId19" xr:uid="{5E9AE83F-97A3-42B4-A896-DBF476BF1841}"/>
-    <hyperlink ref="D28" r:id="rId20" xr:uid="{3CAFCF79-5B81-469C-9B81-FC706CBBFC22}"/>
-    <hyperlink ref="D29" r:id="rId21" xr:uid="{16B91F1D-EBE7-4520-A09B-7D04E3768BAB}"/>
-    <hyperlink ref="D9" r:id="rId22" xr:uid="{EF73ACEF-55E6-4C47-855A-AED01217D904}"/>
+    <hyperlink ref="D23" r:id="rId9" xr:uid="{DEC581DC-25E8-4D22-85FE-968AA311BC4C}"/>
+    <hyperlink ref="D25" r:id="rId10" xr:uid="{25DFE2B8-7111-42E9-BED2-6FAA0E70689C}"/>
+    <hyperlink ref="D26" r:id="rId11" xr:uid="{2B8A48F5-F547-4C41-BD57-626BC8383E02}"/>
+    <hyperlink ref="D27" r:id="rId12" xr:uid="{7D21E112-C538-4EF1-832F-FADEF8B53DBE}"/>
+    <hyperlink ref="D28" r:id="rId13" xr:uid="{8C7FC700-CCF5-4222-ACD9-9FC734098BD2}"/>
+    <hyperlink ref="B27" r:id="rId14" xr:uid="{48C21483-6CA4-4763-AAB2-890458D45A79}"/>
+    <hyperlink ref="B26" r:id="rId15" xr:uid="{9B31FCF5-B1F7-4954-A0D7-C49F11918E5B}"/>
+    <hyperlink ref="D29" r:id="rId16" xr:uid="{4650665B-2233-495D-9E1E-E2BEBDEA1A78}"/>
+    <hyperlink ref="D30" r:id="rId17" xr:uid="{4D8E8BE5-121B-4C5C-979C-7919982CFF66}"/>
+    <hyperlink ref="D31" r:id="rId18" xr:uid="{5E9AE83F-97A3-42B4-A896-DBF476BF1841}"/>
+    <hyperlink ref="D32" r:id="rId19" xr:uid="{3CAFCF79-5B81-469C-9B81-FC706CBBFC22}"/>
+    <hyperlink ref="D33" r:id="rId20" xr:uid="{16B91F1D-EBE7-4520-A09B-7D04E3768BAB}"/>
+    <hyperlink ref="D9" r:id="rId21" xr:uid="{EF73ACEF-55E6-4C47-855A-AED01217D904}"/>
+    <hyperlink ref="D10" r:id="rId22" xr:uid="{AD80B249-811D-406D-B562-4224627D8842}"/>
+    <hyperlink ref="D4" r:id="rId23" xr:uid="{C75CA674-BB0B-4179-9544-633A75106152}"/>
+    <hyperlink ref="D11" r:id="rId24" xr:uid="{856E371A-F032-4D3E-8550-2A9C32AC7BE2}"/>
+    <hyperlink ref="D13" r:id="rId25" xr:uid="{3E4673CE-18D4-40F1-BF88-604E51C2A813}"/>
     <hyperlink ref="C8" location="SA_Coaching!A1" display="Safe / Scaled:  Coaching" xr:uid="{922394D4-3CD9-42E8-9788-ECC018C7164C}"/>
+    <hyperlink ref="D14" r:id="rId26" xr:uid="{D9A1869A-BBFC-46F5-8A62-52EC7E0A0EA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -4356,14 +4660,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4426,14 +4730,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4496,14 +4800,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4566,14 +4870,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4636,14 +4940,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4706,14 +5010,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4776,14 +5080,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4847,12 +5151,12 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
     </row>
@@ -4879,11 +5183,11 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="119" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
       <c r="E3" s="39" t="s">
         <v>149</v>
       </c>
@@ -5179,12 +5483,12 @@
       <c r="A1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
       <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5210,11 +5514,11 @@
       <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="120" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
       <c r="E3" s="48" t="s">
         <v>150</v>
       </c>
@@ -5291,11 +5595,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="120" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="120"/>
       <c r="E12" s="48" t="s">
         <v>150</v>
       </c>
@@ -5459,22 +5763,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -5795,13 +6099,13 @@
       <c r="E26" s="70"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
@@ -5943,8 +6247,8 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,28 +6264,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -6306,16 +6610,16 @@
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="98"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
@@ -6433,9 +6737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4382FB-CCDB-4DE4-9683-3A8D07D3F404}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6450,15 +6752,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="114"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="104"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6484,33 +6786,33 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="116" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="98" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="101" t="s">
         <v>263</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="111" t="s">
+      <c r="E4" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="115" t="s">
+      <c r="G4" s="105" t="s">
         <v>269</v>
       </c>
     </row>
@@ -6520,7 +6822,7 @@
     <mergeCell ref="A3:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{506261BB-1887-4269-878D-19C280DF4387}"/>
+    <hyperlink ref="A1" location="'Primary_Career PATH'!A1" display="&lt;&lt; Back" xr:uid="{506261BB-1887-4269-878D-19C280DF4387}"/>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{AEF28BBC-B5F1-473A-BC5F-452539F5FD99}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{DD01F1AB-393C-42A2-B964-B42E93C18C2C}"/>
   </hyperlinks>
@@ -6547,14 +6849,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6619,14 +6921,14 @@
       <c r="A1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6689,13 +6991,13 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
       <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -6838,14 +7140,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6908,14 +7210,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Added new changes with Proxy Settings
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\2_GIT_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3877F6A6-EADC-429C-B212-908244A69B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821EAD2E-141F-4434-ACFD-B332635DD854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
@@ -38,7 +38,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Career PATH'!$A$3:$H$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="210">
   <si>
     <t>SR#</t>
   </si>
@@ -2264,6 +2263,12 @@
   </si>
   <si>
     <t>Developer to Architect</t>
+  </si>
+  <si>
+    <t>KANBAN</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/paths/skills/increasing-efficiency-with-kanban</t>
   </si>
 </sst>
 </file>
@@ -2535,20 +2540,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2710,6 +2711,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3271,15 +3284,15 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="39" style="20" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" style="16" customWidth="1"/>
+    <col min="3" max="3" width="67.140625" style="71" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
@@ -3288,35 +3301,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="68" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3336,231 +3349,236 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="32" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="31" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="25" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="23" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="25" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="25" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="64" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="60" t="s">
         <v>200</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="26" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="64" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="64" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="60" t="s">
         <v>204</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="24"/>
-      <c r="D23" s="30"/>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="15" t="s">
         <v>40</v>
       </c>
       <c r="E25" t="s">
@@ -3569,16 +3587,16 @@
       <c r="G25" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="21" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="70" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3586,8 +3604,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="13"/>
+      <c r="B27" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3595,8 +3613,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="21" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -3604,8 +3622,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="13"/>
+      <c r="B29" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -3653,9 +3671,10 @@
     <hyperlink ref="C22" r:id="rId16" xr:uid="{2310128F-5B6E-4D76-916B-4F9216A64190}"/>
     <hyperlink ref="B22" location="'Professional Scrum'!A1" display="Introduction to Professional Scrum" xr:uid="{B412A61E-A6A3-430D-8A36-914377A0A709}"/>
     <hyperlink ref="C17" r:id="rId17" xr:uid="{C4318D8A-2D8A-42AD-A624-437316AC3131}"/>
+    <hyperlink ref="C23" r:id="rId18" xr:uid="{A4E5E913-0316-4114-A1F4-C653BC2E83E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -3680,14 +3699,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3752,14 +3771,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3822,14 +3841,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3892,14 +3911,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3962,14 +3981,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4019,31 +4038,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="40"/>
-    <col min="2" max="3" width="19.140625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="65.42578125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="28" style="35" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="35" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="35"/>
+    <col min="1" max="1" width="9.140625" style="36"/>
+    <col min="2" max="3" width="19.140625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="65.42578125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="28" style="31" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" style="31" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -4058,272 +4077,272 @@
       <c r="E2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40">
+      <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="51" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="38" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="31" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
+      <c r="A8" s="36">
         <v>2</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="32" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="32" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="32" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="32" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="32" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="40" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="32" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="31" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="32" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="32" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="46" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="32" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="32" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="23" spans="3:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="32" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="32" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="32" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="32" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="27" spans="3:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="32" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="28" spans="3:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="36" t="s">
+      <c r="E28" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="29" spans="3:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="32" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="E30" s="36" t="s">
+      <c r="E30" s="32" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="3:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="E31" s="36" t="s">
+      <c r="E31" s="32" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="32" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4352,247 +4371,247 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="59"/>
-    <col min="2" max="2" width="41.42578125" style="63" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="62" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="55" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="55"/>
+    <col min="1" max="1" width="9.140625" style="55"/>
+    <col min="2" max="2" width="41.42578125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" style="58" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="51" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="51" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="54"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="59">
+      <c r="A3" s="55">
         <v>1</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="60" t="s">
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="56" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="61" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="58" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="52"/>
+      <c r="E5" s="48"/>
     </row>
     <row r="6" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="B6" s="61"/>
-      <c r="C6" s="61" t="s">
+      <c r="B6" s="57"/>
+      <c r="C6" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="58" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61" t="s">
+      <c r="B7" s="57"/>
+      <c r="C7" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="58" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="58" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="48" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="48" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="48" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="66" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="60" t="s">
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="56" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="48" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="48" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="48" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="58" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="51" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="48" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="58" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="48" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="21" spans="3:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="48" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="E22" s="52" t="s">
+      <c r="E22" s="48" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="23" spans="3:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="48" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="58" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="48" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4669,17 +4688,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4705,7 +4724,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="23" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4752,17 +4771,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4788,7 +4807,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="23" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4814,7 +4833,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
@@ -4824,17 +4843,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -4860,7 +4879,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="23" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4890,24 +4909,24 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="58.42578125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="58.42578125" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="1:8" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" s="31" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -4925,91 +4944,91 @@
       <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="44" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="45" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="45" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="45" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="44" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G10" s="49" t="s">
+      <c r="G10" s="45" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="45" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="45" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="45" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="45" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="45" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="45" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="45" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="45" t="s">
         <v>129</v>
       </c>
     </row>
@@ -5046,14 +5065,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5116,14 +5135,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5186,14 +5205,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5256,14 +5275,14 @@
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5306,12 +5325,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d53f460e102142885dbc8938524af06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" xmlns:ns4="c8965576-7528-46e3-a68d-d4bc5141fdaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51dd3132ab51039a0b8a02bab29c14ac" ns3:_="" ns4:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -5534,6 +5547,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5544,23 +5563,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
-    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC42E61D-1BC2-43F5-95E9-ABDA8B3BC8C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5579,6 +5581,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{236AB03D-89C6-4FEB-AC3B-BF68DD4F8BD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c8965576-7528-46e3-a68d-d4bc5141fdaa"/>
+    <ds:schemaRef ds:uri="df3f84f5-0dce-435a-abac-67420900ba59"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
New Modification & new document added
</commit_message>
<xml_diff>
--- a/Action_Plans_for_learning.xlsx
+++ b/Action_Plans_for_learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\2_GIT_Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB673DD-B38B-4E12-8843-C698ABEF3F94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5533669-A99C-4C91-AB27-576E652E5EEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="933" xr2:uid="{D2D167CA-DC28-4176-B005-81E9223B1EED}"/>
   </bookViews>
@@ -3372,7 +3372,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5582,6 +5582,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d53f460e102142885dbc8938524af06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" xmlns:ns4="c8965576-7528-46e3-a68d-d4bc5141fdaa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51dd3132ab51039a0b8a02bab29c14ac" ns3:_="" ns4:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -5804,15 +5813,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5820,6 +5820,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC42E61D-1BC2-43F5-95E9-ABDA8B3BC8C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5834,14 +5842,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC37F108-450B-470C-B7B9-209E1FAF9670}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>